<commit_message>
Updated maed the 16th Apr 2024. Plenty of modifications, follow report in the .txt file. Also set of instructions in word of how to keep your toolbox updated from matlab
</commit_message>
<xml_diff>
--- a/Data_example/DY103/Sensors_and_Moorings/CTD/Autosal Data/DY103_SALFORM_.xlsx
+++ b/Data_example/DY103/Sensors_and_Moorings/CTD/Autosal Data/DY103_SALFORM_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablotrucco/Documents/Github/PAP_biogeochemical_QC_calibration/Data_example/DY103/Sensors_and_Moorings/CTD/Autosal Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B649A9FC-E6D0-F34F-9240-501D690F7601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4CA260-6241-E247-AAF1-72A046299F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48080" yWindow="-14600" windowWidth="19120" windowHeight="21600" tabRatio="598" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48080" yWindow="-14100" windowWidth="19120" windowHeight="21100" tabRatio="598" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet18" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="Sheet15" sheetId="17" r:id="rId17"/>
     <sheet name="Sheet16" sheetId="18" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5274,7 +5274,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9:D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>